<commit_message>
Presentation control in progress
</commit_message>
<xml_diff>
--- a/public/presentation/content.xlsx
+++ b/public/presentation/content.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA98675-9AAC-47D6-A1FB-B7536F6C5BFB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D29025D-DC4E-43C2-B418-073822410E69}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="0" windowWidth="21690" windowHeight="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="0" windowWidth="21690" windowHeight="240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sequence" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,13 @@
     <sheet name="layers" sheetId="8" r:id="rId3"/>
     <sheet name="menus" sheetId="10" r:id="rId4"/>
     <sheet name="settings" sheetId="6" r:id="rId5"/>
-    <sheet name="johnsonsPopup1" sheetId="11" r:id="rId6"/>
-    <sheet name="johnsonsInfo" sheetId="12" r:id="rId7"/>
-    <sheet name="&lt;Справочник&gt;" sheetId="5" r:id="rId8"/>
+    <sheet name="cycleBookInfo" sheetId="13" r:id="rId6"/>
+    <sheet name="johnsonsPopup1" sheetId="11" r:id="rId7"/>
+    <sheet name="johnsonsInfo" sheetId="12" r:id="rId8"/>
+    <sheet name="&lt;Справочник&gt;" sheetId="5" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="163">
   <si>
     <t>id</t>
   </si>
@@ -74,9 +75,6 @@
     <t>next</t>
   </si>
   <si>
-    <t>controls</t>
-  </si>
-  <si>
     <t>background</t>
   </si>
   <si>
@@ -434,9 +432,6 @@
     <t>{templatePath}menu</t>
   </si>
   <si>
-    <t>{templatePath}controls&gt;Template</t>
-  </si>
-  <si>
     <t>{templatePath}titles</t>
   </si>
   <si>
@@ -468,6 +463,63 @@
   </si>
   <si>
     <t>#red</t>
+  </si>
+  <si>
+    <t>topmenu</t>
+  </si>
+  <si>
+    <t>{templatePath}topmenu</t>
+  </si>
+  <si>
+    <t>maintitle</t>
+  </si>
+  <si>
+    <t>{templatePath}maintitle</t>
+  </si>
+  <si>
+    <t>disable</t>
+  </si>
+  <si>
+    <t>Деактивировать строку</t>
+  </si>
+  <si>
+    <t>столбец, в котором 1 означает - не использовать данную строку</t>
+  </si>
+  <si>
+    <t>CYCLE BOOK</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>с 1 января по 28 февраля</t>
+  </si>
+  <si>
+    <t>leftmenu</t>
+  </si>
+  <si>
+    <t>{templatePath}leftmenu&gt;Template</t>
+  </si>
+  <si>
+    <t>prevnav</t>
+  </si>
+  <si>
+    <t>nextnav</t>
+  </si>
+  <si>
+    <t>{templatePath}prevnav</t>
+  </si>
+  <si>
+    <t>{templatePath}nextnav</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>margin</t>
+  </si>
+  <si>
+    <t>l70</t>
   </si>
 </sst>
 </file>
@@ -603,7 +655,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -648,6 +700,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -953,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -974,7 +1029,7 @@
     <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -982,25 +1037,25 @@
         <v>10</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="H1" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>8</v>
@@ -1008,8 +1063,11 @@
       <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -1017,105 +1075,105 @@
         <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="12" t="s">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="B8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -1123,10 +1181,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>2</v>
       </c>
@@ -1134,10 +1192,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>3</v>
       </c>
@@ -1145,10 +1203,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>4</v>
       </c>
@@ -1156,10 +1214,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>5</v>
       </c>
@@ -1167,10 +1225,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>6</v>
       </c>
@@ -1178,7 +1236,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>1</v>
@@ -1192,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F02F3F-96B3-48BA-B13D-EB6706FA6D0F}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1206,90 +1264,93 @@
     <col min="9" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>15</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>7</v>
@@ -1303,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E4B767-F738-4DC0-AA9C-8AED7BB104BD}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1317,143 +1378,239 @@
     <col min="4" max="4" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" style="8" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" style="8" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="8" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" style="8"/>
-    <col min="17" max="17" width="35" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="8"/>
+    <col min="7" max="7" width="9.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="6" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" style="8" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" style="8" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="8"/>
+    <col min="18" max="18" width="35" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="I6" s="8">
+        <v>70</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="D7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="G7" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="H7" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="H8" s="8">
+        <v>141</v>
+      </c>
+      <c r="I8" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I10" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" s="8">
+        <v>30</v>
+      </c>
+      <c r="I11" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="8">
+        <v>30</v>
+      </c>
+      <c r="I12" s="8">
         <v>100</v>
       </c>
     </row>
@@ -1495,13 +1652,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1509,24 +1666,24 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="8">
         <v>2</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>7</v>
@@ -1534,108 +1691,108 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="8">
         <v>-1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="8">
         <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="8">
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="8">
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1661,31 +1818,31 @@
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="8">
         <v>1280</v>
@@ -1693,7 +1850,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="8">
         <v>720</v>
@@ -1701,7 +1858,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="8">
         <v>1280</v>
@@ -1709,7 +1866,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="8">
         <v>960</v>
@@ -1717,7 +1874,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -1725,7 +1882,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -1733,7 +1890,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="8">
         <v>18</v>
@@ -1741,18 +1898,18 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1762,6 +1919,72 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07CFF63-8A61-4EC8-9286-C73858C2C756}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="135.42578125" style="21" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560EBD8E-A245-488A-9C11-9F9F721470B5}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1782,32 +2005,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>99</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1816,7 +2039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC0A1BD-4758-4764-BE1D-354A27BA823A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1837,32 +2060,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>99</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1871,12 +2094,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1898,13 +2121,13 @@
     </row>
     <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1912,59 +2135,59 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1972,70 +2195,77 @@
     </row>
     <row r="16" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="A26" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>

</xml_diff>

<commit_message>
Navigation and switchable layers
</commit_message>
<xml_diff>
--- a/public/presentation/content.xlsx
+++ b/public/presentation/content.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A0E1C4-DF46-4308-8273-BC355A914BFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DADFEF-5EA1-4476-B09A-7C2F61ECF139}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="0" windowWidth="21690" windowHeight="240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="156">
   <si>
     <t>id</t>
   </si>
@@ -426,9 +426,6 @@
     <t>height</t>
   </si>
   <si>
-    <t>bottom,left</t>
-  </si>
-  <si>
     <t>top,left</t>
   </si>
   <si>
@@ -471,9 +468,6 @@
     <t>leftmenu</t>
   </si>
   <si>
-    <t>{templatePath}leftmenu&gt;Template</t>
-  </si>
-  <si>
     <t>prevnav</t>
   </si>
   <si>
@@ -502,6 +496,9 @@
   </si>
   <si>
     <t>master</t>
+  </si>
+  <si>
+    <t>{templatePath}leftmenu</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1019,7 @@
         <v>24</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>12</v>
@@ -1046,7 +1043,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1057,7 +1054,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1085,10 +1082,10 @@
         <v>18</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>89</v>
@@ -1201,7 +1198,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>11</v>
@@ -1254,7 +1251,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>14</v>
@@ -1269,13 +1266,13 @@
         <v>13</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1292,7 +1289,7 @@
         <v>25</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>42</v>
@@ -1355,7 +1352,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1400,7 +1397,7 @@
         <v>113</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>129</v>
@@ -1409,10 +1406,10 @@
         <v>130</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1464,22 +1461,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H6" s="8">
+        <v>30</v>
       </c>
       <c r="I6" s="8">
-        <v>70</v>
-      </c>
-      <c r="J6" s="8">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1487,19 +1487,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="H7" s="8">
-        <v>70</v>
+        <v>30</v>
+      </c>
+      <c r="I7" s="8">
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1507,16 +1510,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>137</v>
+        <v>93</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
       </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
       <c r="F8" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I8" s="8">
-        <v>70</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1524,18 +1530,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>14</v>
+        <v>144</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I9" s="8">
+        <v>131</v>
+      </c>
+      <c r="H9" s="8">
         <v>70</v>
       </c>
     </row>
@@ -1544,16 +1550,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="8" t="s">
         <v>136</v>
       </c>
       <c r="D10" s="8">
         <v>1</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I10" s="8">
         <v>70</v>
@@ -1564,25 +1567,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="D11" s="8">
         <v>1</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="H11" s="8">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="I11" s="8">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1590,22 +1587,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D12" s="8">
         <v>1</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H12" s="8">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="I12" s="8">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1947,7 +1941,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1966,10 +1960,10 @@
         <v>24</v>
       </c>
       <c r="B4" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>143</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2250,15 +2244,15 @@
     </row>
     <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Version 1.1 with OMOBUS, bugfixes
</commit_message>
<xml_diff>
--- a/public/presentation/content.xlsx
+++ b/public/presentation/content.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AFFE6F-6FC5-4096-9C83-2956081A254D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A06161C-0A6A-4A38-A6EF-EFE160FCDB40}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="0" windowWidth="21690" windowHeight="240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="0" windowWidth="21690" windowHeight="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sequence" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="237">
   <si>
     <t>id</t>
   </si>
@@ -39,12 +39,6 @@
     <t>intro</t>
   </si>
   <si>
-    <t>hexoral02</t>
-  </si>
-  <si>
-    <t>hexoral03</t>
-  </si>
-  <si>
     <t>hexoral</t>
   </si>
   <si>
@@ -102,12 +96,6 @@
     <t>tyzine</t>
   </si>
   <si>
-    <t>Гексорал&lt;sup&gt;®&lt;/sup&gt;</t>
-  </si>
-  <si>
-    <t>Доктор Мом&lt;sup&gt;®&lt;/sup&gt;</t>
-  </si>
-  <si>
     <t>popup1</t>
   </si>
   <si>
@@ -327,12 +315,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>с 1 января по 28 февраля</t>
-  </si>
-  <si>
-    <t>leftmenu</t>
-  </si>
-  <si>
     <t>prevnav</t>
   </si>
   <si>
@@ -351,75 +333,24 @@
     <t>margin</t>
   </si>
   <si>
-    <t>l70</t>
-  </si>
-  <si>
     <t>detailing</t>
   </si>
   <si>
     <t>master</t>
   </si>
   <si>
-    <t>{templatePath}leftmenu</t>
-  </si>
-  <si>
-    <t>hexoral04</t>
-  </si>
-  <si>
     <t>detailingTemplate</t>
   </si>
   <si>
     <t>{slidesPath}detailing&gt;</t>
   </si>
   <si>
-    <t>Мультизима</t>
-  </si>
-  <si>
-    <t>Тизин&lt;sup&gt;®&lt;/sup&gt;</t>
-  </si>
-  <si>
-    <t>Ринза&lt;sup&gt;®&lt;/sup&gt;</t>
-  </si>
-  <si>
     <t>rinza</t>
   </si>
   <si>
     <t>tyzineTemplate</t>
   </si>
   <si>
-    <t>tyzine02</t>
-  </si>
-  <si>
-    <t>tyzine03</t>
-  </si>
-  <si>
-    <t>tyzine04</t>
-  </si>
-  <si>
-    <t>tyzine05</t>
-  </si>
-  <si>
-    <t>{slidesPath}tyzine/002</t>
-  </si>
-  <si>
-    <t>{slidesPath}tyzine/003</t>
-  </si>
-  <si>
-    <t>{slidesPath}tyzine/004</t>
-  </si>
-  <si>
-    <t>{slidesPath}tyzine/005</t>
-  </si>
-  <si>
-    <t>{slidesPath}tyzine&gt;001.jpg</t>
-  </si>
-  <si>
-    <t>{slidesPath}tyzine/005p</t>
-  </si>
-  <si>
-    <t>{templatePath}brandtitle</t>
-  </si>
-  <si>
     <t>&gt;tyzine</t>
   </si>
   <si>
@@ -444,109 +375,373 @@
     <t>&gt;hexoral</t>
   </si>
   <si>
-    <t>{slidesPath}hexoral&gt;001.jpg</t>
-  </si>
-  <si>
-    <t>{slidesPath}hexoral/002</t>
-  </si>
-  <si>
-    <t>{slidesPath}hexoral/003</t>
-  </si>
-  <si>
-    <t>{slidesPath}hexoral/004</t>
-  </si>
-  <si>
-    <t>{slidesPath}hexoral/003p</t>
-  </si>
-  <si>
     <t>doctormom</t>
   </si>
   <si>
-    <t>doctormom02</t>
-  </si>
-  <si>
-    <t>doctormom03</t>
-  </si>
-  <si>
-    <t>doctormom04</t>
-  </si>
-  <si>
-    <t>doctormom05</t>
-  </si>
-  <si>
     <t>doctormomTemplate</t>
   </si>
   <si>
-    <t>{slidesPath}doctormom&gt;001.jpg</t>
-  </si>
-  <si>
-    <t>{slidesPath}doctormom/002</t>
-  </si>
-  <si>
-    <t>{slidesPath}doctormom/003</t>
-  </si>
-  <si>
-    <t>{slidesPath}doctormom/004</t>
-  </si>
-  <si>
-    <t>{slidesPath}doctormom/005</t>
-  </si>
-  <si>
     <t>&gt;doctormom</t>
   </si>
   <si>
-    <t>{slidesPath}doctormom/003p</t>
-  </si>
-  <si>
-    <t>{slidesPath}doctormom/002p</t>
-  </si>
-  <si>
-    <t>rinza02</t>
-  </si>
-  <si>
-    <t>rinza03</t>
-  </si>
-  <si>
-    <t>rinza04</t>
-  </si>
-  <si>
     <t>rinzaTemplate</t>
   </si>
   <si>
-    <t>{slidesPath}rinza&gt;001.jpg</t>
-  </si>
-  <si>
-    <t>{slidesPath}rinza/002</t>
-  </si>
-  <si>
-    <t>{slidesPath}rinza/003</t>
-  </si>
-  <si>
-    <t>{slidesPath}rinza/004</t>
-  </si>
-  <si>
-    <t>{slidesPath}rinza/002p</t>
-  </si>
-  <si>
-    <t>{slidesPath}rinza/003p</t>
-  </si>
-  <si>
-    <t>{slidesPath}rinza/004p</t>
-  </si>
-  <si>
-    <t>multiwinter</t>
-  </si>
-  <si>
     <t>commonTemplate</t>
   </si>
   <si>
-    <t>{slidesPath}multiwinter&gt;002.jpg</t>
-  </si>
-  <si>
-    <t>{slidesPath}multiwinter/001</t>
-  </si>
-  <si>
     <t>&gt;rinza</t>
+  </si>
+  <si>
+    <t>Академия+</t>
+  </si>
+  <si>
+    <t>academyPlus</t>
+  </si>
+  <si>
+    <t>Мотрин&lt;sup&gt;®&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>Микролакс&lt;sup&gt;®&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>Мотилегаз&lt;sup&gt;®&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>Никоретте&lt;sup&gt;®&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>motrine</t>
+  </si>
+  <si>
+    <t>microlax</t>
+  </si>
+  <si>
+    <t>motilegas</t>
+  </si>
+  <si>
+    <t>nicorette</t>
+  </si>
+  <si>
+    <t>{slidesPath}academyPlus/001</t>
+  </si>
+  <si>
+    <t>{slidesPath}academyPlus/002</t>
+  </si>
+  <si>
+    <t>multibrand</t>
+  </si>
+  <si>
+    <t>{slidesPath}multibrand/001</t>
+  </si>
+  <si>
+    <t>motrineTemplate</t>
+  </si>
+  <si>
+    <t>&gt;motrine</t>
+  </si>
+  <si>
+    <t>microlaxTemplate</t>
+  </si>
+  <si>
+    <t>&gt;microlax</t>
+  </si>
+  <si>
+    <t>motilegasTemplate</t>
+  </si>
+  <si>
+    <t>&gt;motilegas</t>
+  </si>
+  <si>
+    <t>nicoretteTemplate</t>
+  </si>
+  <si>
+    <t>&gt;nicorette</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>с 1 ноября по 31 декабря</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/002</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/003</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/004</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/005</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/005p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/001</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/002p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/003p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/004p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/006</t>
+  </si>
+  <si>
+    <t>{slidesPath}motrine/006p</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/001</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/002</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/003</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/004</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/005</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/006</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/007</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/008</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/002p</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/003p</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/004p</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/005p</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/006p</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/007p</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/008p</t>
+  </si>
+  <si>
+    <t>{slidesPath}microlax/005pp</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/001</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/002</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/003</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/004</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/005</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/006</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/007</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/008</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/002p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/004p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/005p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/006p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/007p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/008p</t>
+  </si>
+  <si>
+    <t>{slidesPath}motilegas/005pp</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/001</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/002</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/003</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/004</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/005</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/006</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/007</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/002p</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/002pp</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/003p</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/004p</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/005p</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/006p</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/007p</t>
+  </si>
+  <si>
+    <t>{slidesPath}nicorette/006pp</t>
+  </si>
+  <si>
+    <t>{slidesPath}multibrand/002</t>
+  </si>
+  <si>
+    <t>motrine2</t>
+  </si>
+  <si>
+    <t>motrine3</t>
+  </si>
+  <si>
+    <t>motrine4</t>
+  </si>
+  <si>
+    <t>motrine5</t>
+  </si>
+  <si>
+    <t>motrine6</t>
+  </si>
+  <si>
+    <t>microlax2</t>
+  </si>
+  <si>
+    <t>microlax3</t>
+  </si>
+  <si>
+    <t>microlax4</t>
+  </si>
+  <si>
+    <t>microlax5</t>
+  </si>
+  <si>
+    <t>microlax6</t>
+  </si>
+  <si>
+    <t>microlax7</t>
+  </si>
+  <si>
+    <t>microlax8</t>
+  </si>
+  <si>
+    <t>motilegas2</t>
+  </si>
+  <si>
+    <t>motilegas3</t>
+  </si>
+  <si>
+    <t>motilegas4</t>
+  </si>
+  <si>
+    <t>motilegas5</t>
+  </si>
+  <si>
+    <t>motilegas6</t>
+  </si>
+  <si>
+    <t>motilegas7</t>
+  </si>
+  <si>
+    <t>motilegas8</t>
+  </si>
+  <si>
+    <t>nicorette2</t>
+  </si>
+  <si>
+    <t>nicorette3</t>
+  </si>
+  <si>
+    <t>nicorette4</t>
+  </si>
+  <si>
+    <t>nicorette6</t>
+  </si>
+  <si>
+    <t>nicorette5</t>
+  </si>
+  <si>
+    <t>nicorette7</t>
+  </si>
+  <si>
+    <t>multibrand2</t>
+  </si>
+  <si>
+    <t>academyPlus3</t>
+  </si>
+  <si>
+    <t>extra</t>
+  </si>
+  <si>
+    <t>l0,t-320</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>{theme:"dark"}</t>
+  </si>
+  <si>
+    <t>exitpopup</t>
+  </si>
+  <si>
+    <t>{templatePath}exitpopup</t>
+  </si>
+  <si>
+    <t>{theme:"light", prev:"disabled",home:"disabled"}</t>
+  </si>
+  <si>
+    <t>academyPlus02</t>
   </si>
 </sst>
 </file>
@@ -556,7 +751,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,8 +819,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -692,6 +893,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -707,7 +914,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -764,6 +971,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1067,315 +1279,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="26" style="8" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="8"/>
+    <col min="5" max="5" width="25.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.85546875" style="8" customWidth="1"/>
+    <col min="9" max="9" width="26" style="8" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="J4" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
-        <v>116</v>
+      <c r="J17" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
+        <v>211</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
-        <v>156</v>
+      <c r="D18" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>212</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>161</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
-        <v>157</v>
+        <v>168</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>213</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>162</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>158</v>
+        <v>169</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>128</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
-        <v>167</v>
+        <v>171</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>214</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F22" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="14" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1387,10 +1975,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F02F3F-96B3-48BA-B13D-EB6706FA6D0F}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1403,120 +1991,164 @@
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>107</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1527,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E4B767-F738-4DC0-AA9C-8AED7BB104BD}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1557,37 +2189,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="J1" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
@@ -1595,10 +2227,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J2" s="25">
         <v>1</v>
@@ -1609,7 +2241,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K3" s="8">
         <v>1</v>
@@ -1620,23 +2252,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24">
+    <row r="5" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="25">
-        <v>1</v>
-      </c>
-      <c r="J5" s="25">
+      <c r="B5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="30">
         <v>1</v>
       </c>
     </row>
@@ -1645,25 +2274,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="H6" s="8">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="I6" s="8">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1671,22 +2297,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H7" s="8">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="I7" s="8">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1694,19 +2320,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>88</v>
+      <c r="G8" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="I8" s="8">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1714,19 +2340,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
       </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
       <c r="F9" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="8">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1734,39 +2360,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>12</v>
+        <v>233</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="D10" s="8">
         <v>1</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="8">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="E10" s="8">
         <v>1</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="8">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1779,7 +2382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADBD7ED-DDEE-48B2-ACB4-DB3359AEA9DF}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1807,13 +2410,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1821,57 +2424,57 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1885,7 +2488,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1897,31 +2500,31 @@
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" s="8">
         <v>1280</v>
@@ -1929,7 +2532,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" s="8">
         <v>720</v>
@@ -1937,7 +2540,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B6" s="8">
         <v>1280</v>
@@ -1945,7 +2548,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" s="8">
         <v>960</v>
@@ -1953,7 +2556,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -1961,7 +2564,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -1969,7 +2572,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B10" s="8">
         <v>18</v>
@@ -1977,23 +2580,23 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="B13" s="8">
         <v>0</v>
@@ -2001,7 +2604,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B14" s="8">
         <v>5</v>
@@ -2009,7 +2612,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="B15" s="21">
         <v>0</v>
@@ -2017,7 +2620,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="B16" s="8">
         <v>0.7</v>
@@ -2025,10 +2628,10 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2042,7 +2645,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2058,48 +2661,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="22">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2124,32 +2730,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2179,32 +2785,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2217,8 +2823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2240,13 +2846,13 @@
     </row>
     <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2254,59 +2860,59 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2314,76 +2920,76 @@
     </row>
     <row r="16" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
open link function added
</commit_message>
<xml_diff>
--- a/public/presentation/content.xlsx
+++ b/public/presentation/content.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BEC8D9-E8FE-498D-A2EA-23B32C4B266C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F44D2AB-D449-4F45-BCDB-6265A86D5E86}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="0" windowWidth="21690" windowHeight="240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="0" windowWidth="21690" windowHeight="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sequence" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="229">
   <si>
     <t>id</t>
   </si>
@@ -372,9 +372,6 @@
     <t>{slidesPath}academyPlus/001</t>
   </si>
   <si>
-    <t>{slidesPath}academyPlus/002</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -552,9 +549,6 @@
     <t>{slidesPath}multibrand/002</t>
   </si>
   <si>
-    <t>academyPlus2</t>
-  </si>
-  <si>
     <t>motrine2</t>
   </si>
   <si>
@@ -639,9 +633,6 @@
     <t>extra</t>
   </si>
   <si>
-    <t>l0,t-320</t>
-  </si>
-  <si>
     <t>home</t>
   </si>
   <si>
@@ -663,33 +654,6 @@
     <t>popup5</t>
   </si>
   <si>
-    <t>academyPlus4</t>
-  </si>
-  <si>
-    <t>academyPlus5</t>
-  </si>
-  <si>
-    <t>academyPlus6</t>
-  </si>
-  <si>
-    <t>academyPlus7</t>
-  </si>
-  <si>
-    <t>{slidesPath}academyPlus/003</t>
-  </si>
-  <si>
-    <t>{slidesPath}academyPlus/004</t>
-  </si>
-  <si>
-    <t>{slidesPath}academyPlus/005</t>
-  </si>
-  <si>
-    <t>{slidesPath}academyPlus/006</t>
-  </si>
-  <si>
-    <t>{slidesPath}academyPlus/007</t>
-  </si>
-  <si>
     <t>{theme:"academy", prev:"disabled",home:"disabled"}</t>
   </si>
   <si>
@@ -700,6 +664,60 @@
   </si>
   <si>
     <t>{slidesPath}virus/001</t>
+  </si>
+  <si>
+    <t>Academy Plus</t>
+  </si>
+  <si>
+    <t>{slidesPath}academy/001</t>
+  </si>
+  <si>
+    <t>{slidesPath}academy/002</t>
+  </si>
+  <si>
+    <t>{slidesPath}academy/003</t>
+  </si>
+  <si>
+    <t>{slidesPath}academy/004</t>
+  </si>
+  <si>
+    <t>{slidesPath}academy/005</t>
+  </si>
+  <si>
+    <t>{slidesPath}academy/006</t>
+  </si>
+  <si>
+    <t>{slidesPath}academy/007</t>
+  </si>
+  <si>
+    <t>l0,t-600</t>
+  </si>
+  <si>
+    <t>{slidesPath}academy/001p</t>
+  </si>
+  <si>
+    <t>academy</t>
+  </si>
+  <si>
+    <t>academy2</t>
+  </si>
+  <si>
+    <t>academy3</t>
+  </si>
+  <si>
+    <t>academy4</t>
+  </si>
+  <si>
+    <t>academy5</t>
+  </si>
+  <si>
+    <t>academy6</t>
+  </si>
+  <si>
+    <t>academy7</t>
+  </si>
+  <si>
+    <t>{theme:"academy",link1:{url:"https://forms.office.com/r/5zASR1k4NT",target:"_blank"}}</t>
   </si>
 </sst>
 </file>
@@ -1234,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1245,19 +1263,20 @@
     <col min="1" max="1" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="8" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.85546875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="26" style="8" customWidth="1"/>
-    <col min="10" max="10" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" style="8" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="8"/>
+    <col min="4" max="4" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="21.85546875" style="8" customWidth="1"/>
+    <col min="13" max="13" width="26" style="8" customWidth="1"/>
+    <col min="14" max="14" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.5703125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" style="8" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1271,267 +1290,294 @@
         <v>16</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="F1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="L1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>173</v>
+        <v>222</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="J3" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="L3" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N3" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="K4" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L4" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="J5" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L5" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="K6" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L6" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="J7" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L7" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="K8" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="L8" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N8" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="F9" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="J9" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N9" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="B12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="B13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="B14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N14" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
         <v>109</v>
       </c>
@@ -1539,141 +1585,141 @@
         <v>101</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="D16" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
+      <c r="B18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
+      <c r="B19" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+      <c r="B20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="B21" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N22" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
         <v>110</v>
       </c>
@@ -1681,138 +1727,138 @@
         <v>101</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="F23" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
+      <c r="D24" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="8" t="s">
+      <c r="B26" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+      <c r="N26" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
+      <c r="B27" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
+      <c r="B28" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
+      <c r="B29" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="8" t="s">
+      <c r="B30" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="J29" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N30" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>111</v>
       </c>
@@ -1820,131 +1866,131 @@
         <v>101</v>
       </c>
       <c r="C31" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="N31" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F31" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
+      <c r="D32" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="K32" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="N32" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="N33" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
+      <c r="B34" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
+      <c r="B36" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E36" s="8" t="s">
+      <c r="B38" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
+      <c r="J38" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="27" t="s">
         <v>198</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="27" t="s">
-        <v>200</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>101</v>
@@ -1952,7 +1998,7 @@
       <c r="C39" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G39" s="14" t="s">
+      <c r="K39" s="14" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1964,10 +2010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F02F3F-96B3-48BA-B13D-EB6706FA6D0F}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2023,6 +2069,14 @@
         <v>101</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -2034,7 +2088,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2124,7 +2178,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
@@ -2161,7 +2215,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -2174,7 +2228,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -2187,7 +2241,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E9" s="29">
         <v>1</v>
@@ -2210,10 +2264,10 @@
         <v>76</v>
       </c>
       <c r="H10" s="8">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="I10" s="8">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -2233,10 +2287,10 @@
         <v>92</v>
       </c>
       <c r="H11" s="8">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="I11" s="8">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -2253,10 +2307,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="I12" s="8">
-        <v>60</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -2284,10 +2338,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D14" s="8">
         <v>1</v>
@@ -2412,7 +2466,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2451,7 +2505,7 @@
         <v>63</v>
       </c>
       <c r="B4" s="8">
-        <v>1280</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2459,7 +2513,7 @@
         <v>64</v>
       </c>
       <c r="B5" s="8">
-        <v>720</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2467,7 +2521,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="8">
-        <v>1280</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2475,7 +2529,7 @@
         <v>62</v>
       </c>
       <c r="B7" s="8">
-        <v>960</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2610,7 +2664,7 @@
         <v>51</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2621,7 +2675,7 @@
         <v>87</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New slide types added
</commit_message>
<xml_diff>
--- a/public/presentation/content.xlsx
+++ b/public/presentation/content.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E625963-6E8B-45AA-A255-FF611C1B81C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613B0B91-B4B3-4C70-BB96-6C2E5800AB85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="0" windowWidth="21690" windowHeight="240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="0" windowWidth="21690" windowHeight="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sequence" sheetId="1" r:id="rId1"/>
-    <sheet name="templates" sheetId="9" r:id="rId2"/>
+    <sheet name="menus" sheetId="10" r:id="rId2"/>
     <sheet name="layers" sheetId="8" r:id="rId3"/>
-    <sheet name="menus" sheetId="10" r:id="rId4"/>
+    <sheet name="templates" sheetId="9" r:id="rId4"/>
     <sheet name="settings" sheetId="6" r:id="rId5"/>
     <sheet name="&lt;Справочник&gt;" sheetId="5" r:id="rId6"/>
   </sheets>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="263">
   <si>
     <t>id</t>
   </si>
@@ -78,9 +78,6 @@
     <t>popup1</t>
   </si>
   <si>
-    <t>popup2</t>
-  </si>
-  <si>
     <t>Источник контента</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
     <t>academyPlus</t>
   </si>
   <si>
-    <t>extra</t>
-  </si>
-  <si>
     <t>home</t>
   </si>
   <si>
@@ -327,9 +321,6 @@
     <t>{templatePath}exitpopup</t>
   </si>
   <si>
-    <t>{theme:"academy", prev:"disabled",home:"disabled"}</t>
-  </si>
-  <si>
     <t>virus</t>
   </si>
   <si>
@@ -384,9 +375,6 @@
     <t>academy7</t>
   </si>
   <si>
-    <t>{theme:"academy",link1:{url:"https://forms.office.com/r/5zASR1k4NT",target:"_blank"}}</t>
-  </si>
-  <si>
     <t>virus2</t>
   </si>
   <si>
@@ -660,9 +648,6 @@
     <t>Tyzine</t>
   </si>
   <si>
-    <t>{theme:"dark",home:"disabled"}</t>
-  </si>
-  <si>
     <t>JNJ Университеты</t>
   </si>
   <si>
@@ -681,12 +666,6 @@
     <t>l0,t-356</t>
   </si>
   <si>
-    <t>{theme:"academy",link1:{url:"https://forms.office.com/r/kDM3T4xHid",target:"_blank"}}</t>
-  </si>
-  <si>
-    <t>{theme:"academy",link1:{url:"https://forms.office.com/r/ZcZzmGGM7y",target:"_blank"}}</t>
-  </si>
-  <si>
     <t>hexoral</t>
   </si>
   <si>
@@ -784,6 +763,60 @@
   </si>
   <si>
     <t>Гексорал&lt;sup&gt;®&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>{theme:"academy",link1:{url:"https://forms.office.com/r/5zASR1k4NT",target:"_blank"},menu:"academy"}</t>
+  </si>
+  <si>
+    <t>{theme:"academy",link1:{url:"https://forms.office.com/r/ZcZzmGGM7y",target:"_blank"},menu:"academy"}</t>
+  </si>
+  <si>
+    <t>{theme:"academy",link1:{url:"https://forms.office.com/r/kDM3T4xHid",target:"_blank"},menu:"academy"}</t>
+  </si>
+  <si>
+    <t>bottommenu</t>
+  </si>
+  <si>
+    <t>{templatePath}bottommenu</t>
+  </si>
+  <si>
+    <t>l0,t356</t>
+  </si>
+  <si>
+    <t>popup</t>
+  </si>
+  <si>
+    <t>{theme:"academy",menu:"academy"}</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>dev2</t>
+  </si>
+  <si>
+    <t>{slidesPath}dev/001</t>
+  </si>
+  <si>
+    <t>{slidesPath}dev/002</t>
+  </si>
+  <si>
+    <t>{slidesPath}dev/001p1</t>
+  </si>
+  <si>
+    <t>{slidesPath}dev/002p1</t>
+  </si>
+  <si>
+    <t>dev3</t>
+  </si>
+  <si>
+    <t>{slidesPath}dev/003p1</t>
+  </si>
+  <si>
+    <t>{slidesPath}dev/003</t>
   </si>
 </sst>
 </file>
@@ -1291,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1302,8 +1335,8 @@
     <col min="1" max="1" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="8" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="21.85546875" style="8" customWidth="1"/>
     <col min="9" max="9" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
@@ -1324,22 +1357,22 @@
         <v>9</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>13</v>
@@ -1351,1164 +1384,1221 @@
         <v>2</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>111</v>
+      <c r="A2" s="23" t="s">
+        <v>254</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>103</v>
+        <v>262</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>100</v>
+        <v>261</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>112</v>
+      <c r="A3" s="23" t="s">
+        <v>255</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>111</v>
+        <v>256</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>258</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
-        <v>113</v>
+      <c r="A4" s="23" t="s">
+        <v>260</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>111</v>
+        <v>257</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>254</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>111</v>
+        <v>100</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>218</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="24" t="s">
-        <v>111</v>
-      </c>
       <c r="H7" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>111</v>
+        <v>103</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>100</v>
+      <c r="A9" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>100</v>
+        <v>104</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>210</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>119</v>
+      <c r="A10" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>100</v>
+        <v>105</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>96</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>120</v>
+      <c r="A11" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>100</v>
+        <v>106</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>96</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>136</v>
+        <v>98</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>125</v>
+      <c r="A16" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
-        <v>126</v>
+      <c r="A17" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>125</v>
+        <v>134</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
-        <v>127</v>
+      <c r="A18" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>125</v>
+        <v>135</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>125</v>
+        <v>145</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>157</v>
+        <v>147</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>158</v>
+        <v>148</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>149</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>159</v>
+        <v>150</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>125</v>
+        <v>152</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>161</v>
+      <c r="A25" s="23" t="s">
+        <v>127</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>124</v>
+        <v>121</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>162</v>
+      <c r="A26" s="23" t="s">
+        <v>128</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
-        <v>163</v>
+      <c r="A27" s="23" t="s">
+        <v>129</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="H27" s="20" t="s">
-        <v>161</v>
+        <v>156</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>161</v>
+        <v>187</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>198</v>
+        <v>191</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>161</v>
+        <v>179</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>194</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>202</v>
+        <v>196</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="13" t="s">
-        <v>219</v>
+      <c r="A40" s="20" t="s">
+        <v>169</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G40" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H40" s="12" t="s">
-        <v>124</v>
+        <v>198</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>215</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="13" t="s">
-        <v>221</v>
+      <c r="A41" s="20" t="s">
+        <v>170</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>219</v>
+        <v>185</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
-        <v>222</v>
+      <c r="A42" s="20" t="s">
+        <v>171</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>219</v>
+        <v>200</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>157</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C43" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="F43" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>219</v>
+      <c r="F43" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="G43" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>96</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2518,112 +2608,168 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F02F3F-96B3-48BA-B13D-EB6706FA6D0F}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADBD7ED-DDEE-48B2-ACB4-DB3359AEA9DF}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="8" customWidth="1"/>
-    <col min="2" max="5" width="27" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="2" width="14.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="28.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="6" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" style="8" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" style="8" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="8" customWidth="1"/>
+    <col min="15" max="16" width="9.140625" style="8"/>
+    <col min="17" max="17" width="35" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="8">
         <v>3</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="D10" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="8">
+        <v>4</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="8">
         <v>6</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>220</v>
+      <c r="D13" s="24" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2637,7 +2783,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A3" sqref="A3:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2673,28 +2819,28 @@
         <v>8</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
@@ -2705,7 +2851,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J2" s="22">
         <v>1</v>
@@ -2726,10 +2872,12 @@
       <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="B4" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2737,13 +2885,20 @@
       <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25">
+      <c r="B5" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="8">
         <v>1</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="I5" s="8">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2751,7 +2906,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>16</v>
+        <v>251</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -2764,16 +2919,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H7" s="8">
         <v>61</v>
@@ -2787,16 +2942,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H8" s="8">
         <v>61</v>
@@ -2810,16 +2965,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I9" s="8">
         <v>61</v>
@@ -2830,10 +2985,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="8">
         <v>1</v>
@@ -2842,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -2850,10 +3005,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D11" s="8">
         <v>1</v>
@@ -2869,102 +3024,112 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADBD7ED-DDEE-48B2-ACB4-DB3359AEA9DF}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F02F3F-96B3-48BA-B13D-EB6706FA6D0F}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="28.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" style="8" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" style="8" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="8" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" style="8"/>
-    <col min="17" max="17" width="35" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="18.5703125" style="8" customWidth="1"/>
+    <col min="2" max="5" width="27" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="8" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>211</v>
+        <v>40</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2978,7 +3143,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2990,31 +3155,31 @@
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="8">
         <v>1280</v>
@@ -3022,7 +3187,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="8">
         <v>800</v>
@@ -3030,7 +3195,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="8">
         <v>1280</v>
@@ -3038,7 +3203,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="8">
         <v>960</v>
@@ -3046,7 +3211,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -3054,7 +3219,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -3062,7 +3227,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="8">
         <v>18</v>
@@ -3070,23 +3235,23 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="8">
         <v>0</v>
@@ -3094,15 +3259,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="19">
         <v>0</v>
@@ -3110,7 +3275,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="8">
         <v>0.7</v>
@@ -3118,10 +3283,10 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3157,13 +3322,13 @@
     </row>
     <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3171,59 +3336,59 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3231,76 +3396,76 @@
     </row>
     <row r="16" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3365,7 +3530,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="1" id="{4D6503AA-0467-49DD-B41C-1AA5E6B69180}">
-            <xm:f>EXACT('C:\ConverterCloud\[clients.xlsx]clients'!#REF!,#REF!)</xm:f>
+            <xm:f>EXACT('\ConverterCloud\[clients.xlsx]clients'!#REF!,#REF!)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>

</xml_diff>